<commit_message>
A few forward tests
</commit_message>
<xml_diff>
--- a/CopterMoveANDLocalisation/CopterMoveAndLocalisation.xlsx
+++ b/CopterMoveANDLocalisation/CopterMoveAndLocalisation.xlsx
@@ -864,6 +864,43 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -912,43 +949,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1236,7 +1236,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>-8.1999999999999993</c:v>
+                  <c:v>-14.4</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1257,7 +1257,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>16.399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1390,7 +1390,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>-6</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1411,7 +1411,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -2332,13 +2332,13 @@
                   <c:v>24.947945807220282</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.456002793295749</c:v>
+                  <c:v>21.824756585125982</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>13.792751719653335</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>11.661903789690601</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7776,8 +7776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AY43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7800,48 +7800,48 @@
   <sheetData>
     <row r="1" spans="2:51" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:51" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="74" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="76" t="s">
+      <c r="B2" s="87" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="76" t="s">
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="76"/>
-      <c r="J2" s="76"/>
-      <c r="K2" s="76"/>
-      <c r="L2" s="76"/>
-      <c r="M2" s="77" t="s">
+      <c r="I2" s="89"/>
+      <c r="J2" s="89"/>
+      <c r="K2" s="89"/>
+      <c r="L2" s="89"/>
+      <c r="M2" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="N2" s="72" t="s">
+      <c r="N2" s="85" t="s">
         <v>19</v>
       </c>
-      <c r="O2" s="62" t="s">
+      <c r="O2" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="P2" s="80" t="s">
+      <c r="P2" s="66" t="s">
         <v>26</v>
       </c>
-      <c r="Q2" s="81"/>
-      <c r="R2" s="81"/>
-      <c r="S2" s="81"/>
-      <c r="T2" s="82"/>
-      <c r="U2" s="78" t="s">
+      <c r="Q2" s="67"/>
+      <c r="R2" s="67"/>
+      <c r="S2" s="67"/>
+      <c r="T2" s="68"/>
+      <c r="U2" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="V2" s="89" t="s">
+      <c r="V2" s="63" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="3" spans="2:51" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="75"/>
+      <c r="B3" s="88"/>
       <c r="C3" s="31" t="s">
         <v>3</v>
       </c>
@@ -7872,51 +7872,51 @@
       <c r="L3" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="75"/>
-      <c r="N3" s="73"/>
-      <c r="O3" s="63"/>
-      <c r="P3" s="83" t="s">
+      <c r="M3" s="88"/>
+      <c r="N3" s="86"/>
+      <c r="O3" s="76"/>
+      <c r="P3" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="Q3" s="83" t="s">
+      <c r="Q3" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="R3" s="83" t="s">
+      <c r="R3" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="S3" s="83" t="s">
+      <c r="S3" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="T3" s="86" t="s">
+      <c r="T3" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="U3" s="79"/>
-      <c r="V3" s="89"/>
+      <c r="U3" s="65"/>
+      <c r="V3" s="63"/>
     </row>
     <row r="4" spans="2:51" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="64" t="s">
+      <c r="B4" s="77" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
-      <c r="F4" s="65"/>
-      <c r="G4" s="65"/>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="65"/>
-      <c r="K4" s="65"/>
-      <c r="L4" s="65"/>
-      <c r="M4" s="65"/>
-      <c r="N4" s="65"/>
-      <c r="O4" s="71"/>
-      <c r="P4" s="84"/>
-      <c r="Q4" s="84"/>
-      <c r="R4" s="84"/>
-      <c r="S4" s="84"/>
-      <c r="T4" s="87"/>
-      <c r="U4" s="79"/>
-      <c r="V4" s="89"/>
+      <c r="C4" s="78"/>
+      <c r="D4" s="78"/>
+      <c r="E4" s="78"/>
+      <c r="F4" s="78"/>
+      <c r="G4" s="78"/>
+      <c r="H4" s="78"/>
+      <c r="I4" s="78"/>
+      <c r="J4" s="78"/>
+      <c r="K4" s="78"/>
+      <c r="L4" s="78"/>
+      <c r="M4" s="78"/>
+      <c r="N4" s="78"/>
+      <c r="O4" s="84"/>
+      <c r="P4" s="70"/>
+      <c r="Q4" s="70"/>
+      <c r="R4" s="70"/>
+      <c r="S4" s="70"/>
+      <c r="T4" s="73"/>
+      <c r="U4" s="65"/>
+      <c r="V4" s="63"/>
     </row>
     <row r="5" spans="2:51" x14ac:dyDescent="0.25">
       <c r="B5" s="18" t="s">
@@ -7944,13 +7944,13 @@
         <f>SQRT(M5*M5+N5*N5)</f>
         <v>0</v>
       </c>
-      <c r="P5" s="84"/>
-      <c r="Q5" s="84"/>
-      <c r="R5" s="84"/>
-      <c r="S5" s="84"/>
-      <c r="T5" s="87"/>
-      <c r="U5" s="79"/>
-      <c r="V5" s="89"/>
+      <c r="P5" s="70"/>
+      <c r="Q5" s="70"/>
+      <c r="R5" s="70"/>
+      <c r="S5" s="70"/>
+      <c r="T5" s="73"/>
+      <c r="U5" s="65"/>
+      <c r="V5" s="63"/>
     </row>
     <row r="6" spans="2:51" x14ac:dyDescent="0.25">
       <c r="B6" s="19" t="s">
@@ -7978,13 +7978,13 @@
         <f t="shared" ref="O6:O33" si="2">SQRT(M6*M6+N6*N6)</f>
         <v>0</v>
       </c>
-      <c r="P6" s="84"/>
-      <c r="Q6" s="84"/>
-      <c r="R6" s="84"/>
-      <c r="S6" s="84"/>
-      <c r="T6" s="87"/>
-      <c r="U6" s="79"/>
-      <c r="V6" s="89"/>
+      <c r="P6" s="70"/>
+      <c r="Q6" s="70"/>
+      <c r="R6" s="70"/>
+      <c r="S6" s="70"/>
+      <c r="T6" s="73"/>
+      <c r="U6" s="65"/>
+      <c r="V6" s="63"/>
     </row>
     <row r="7" spans="2:51" x14ac:dyDescent="0.25">
       <c r="B7" s="19" t="s">
@@ -8012,13 +8012,13 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P7" s="84"/>
-      <c r="Q7" s="84"/>
-      <c r="R7" s="84"/>
-      <c r="S7" s="84"/>
-      <c r="T7" s="87"/>
-      <c r="U7" s="79"/>
-      <c r="V7" s="89"/>
+      <c r="P7" s="70"/>
+      <c r="Q7" s="70"/>
+      <c r="R7" s="70"/>
+      <c r="S7" s="70"/>
+      <c r="T7" s="73"/>
+      <c r="U7" s="65"/>
+      <c r="V7" s="63"/>
     </row>
     <row r="8" spans="2:51" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="20" t="s">
@@ -8046,13 +8046,13 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P8" s="84"/>
-      <c r="Q8" s="84"/>
-      <c r="R8" s="84"/>
-      <c r="S8" s="84"/>
-      <c r="T8" s="87"/>
-      <c r="U8" s="79"/>
-      <c r="V8" s="89"/>
+      <c r="P8" s="70"/>
+      <c r="Q8" s="70"/>
+      <c r="R8" s="70"/>
+      <c r="S8" s="70"/>
+      <c r="T8" s="73"/>
+      <c r="U8" s="65"/>
+      <c r="V8" s="63"/>
       <c r="AK8" s="61"/>
       <c r="AL8" s="61" t="s">
         <v>28</v>
@@ -8067,29 +8067,29 @@
       <c r="AS8" s="61"/>
     </row>
     <row r="9" spans="2:51" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="67" t="s">
+      <c r="B9" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="68"/>
-      <c r="D9" s="68"/>
-      <c r="E9" s="68"/>
-      <c r="F9" s="68"/>
-      <c r="G9" s="68"/>
-      <c r="H9" s="68"/>
-      <c r="I9" s="68"/>
-      <c r="J9" s="68"/>
-      <c r="K9" s="68"/>
-      <c r="L9" s="68"/>
-      <c r="M9" s="68"/>
-      <c r="N9" s="68"/>
-      <c r="O9" s="70"/>
-      <c r="P9" s="85"/>
-      <c r="Q9" s="85"/>
-      <c r="R9" s="85"/>
-      <c r="S9" s="85"/>
-      <c r="T9" s="88"/>
-      <c r="U9" s="79"/>
-      <c r="V9" s="89"/>
+      <c r="C9" s="81"/>
+      <c r="D9" s="81"/>
+      <c r="E9" s="81"/>
+      <c r="F9" s="81"/>
+      <c r="G9" s="81"/>
+      <c r="H9" s="81"/>
+      <c r="I9" s="81"/>
+      <c r="J9" s="81"/>
+      <c r="K9" s="81"/>
+      <c r="L9" s="81"/>
+      <c r="M9" s="81"/>
+      <c r="N9" s="81"/>
+      <c r="O9" s="83"/>
+      <c r="P9" s="71"/>
+      <c r="Q9" s="71"/>
+      <c r="R9" s="71"/>
+      <c r="S9" s="71"/>
+      <c r="T9" s="74"/>
+      <c r="U9" s="65"/>
+      <c r="V9" s="63"/>
       <c r="W9">
         <v>1</v>
       </c>
@@ -8215,10 +8215,10 @@
         <f>AVERAGE(P10:T10)</f>
         <v>33.571257493560516</v>
       </c>
-      <c r="W10" s="90">
+      <c r="W10" s="62">
         <v>1.1805555555555555E-2</v>
       </c>
-      <c r="Y10" s="90">
+      <c r="Y10" s="62">
         <v>1.2499999999999999E-2</v>
       </c>
       <c r="AC10">
@@ -8343,7 +8343,7 @@
         <f t="shared" ref="U11:U33" si="12">AVERAGE(P11:T11)</f>
         <v>0</v>
       </c>
-      <c r="V11" s="90"/>
+      <c r="V11" s="62"/>
       <c r="AC11">
         <v>5</v>
       </c>
@@ -8466,7 +8466,7 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="X12" s="90">
+      <c r="X12" s="62">
         <v>2.013888888888889E-2</v>
       </c>
       <c r="AC12">
@@ -8664,22 +8664,22 @@
       </c>
     </row>
     <row r="14" spans="2:51" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="67" t="s">
+      <c r="B14" s="80" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="68"/>
-      <c r="D14" s="68"/>
-      <c r="E14" s="68"/>
-      <c r="F14" s="68"/>
-      <c r="G14" s="68"/>
-      <c r="H14" s="68"/>
-      <c r="I14" s="68"/>
-      <c r="J14" s="68"/>
-      <c r="K14" s="68"/>
-      <c r="L14" s="68"/>
-      <c r="M14" s="68"/>
-      <c r="N14" s="68"/>
-      <c r="O14" s="69"/>
+      <c r="C14" s="81"/>
+      <c r="D14" s="81"/>
+      <c r="E14" s="81"/>
+      <c r="F14" s="81"/>
+      <c r="G14" s="81"/>
+      <c r="H14" s="81"/>
+      <c r="I14" s="81"/>
+      <c r="J14" s="81"/>
+      <c r="K14" s="81"/>
+      <c r="L14" s="81"/>
+      <c r="M14" s="81"/>
+      <c r="N14" s="81"/>
+      <c r="O14" s="82"/>
       <c r="P14" s="51"/>
       <c r="Q14" s="51"/>
       <c r="R14" s="51"/>
@@ -9084,22 +9084,22 @@
       </c>
     </row>
     <row r="19" spans="2:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="67" t="s">
+      <c r="B19" s="80" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="68"/>
-      <c r="D19" s="68"/>
-      <c r="E19" s="68"/>
-      <c r="F19" s="68"/>
-      <c r="G19" s="68"/>
-      <c r="H19" s="68"/>
-      <c r="I19" s="68"/>
-      <c r="J19" s="68"/>
-      <c r="K19" s="68"/>
-      <c r="L19" s="68"/>
-      <c r="M19" s="68"/>
-      <c r="N19" s="68"/>
-      <c r="O19" s="69"/>
+      <c r="C19" s="81"/>
+      <c r="D19" s="81"/>
+      <c r="E19" s="81"/>
+      <c r="F19" s="81"/>
+      <c r="G19" s="81"/>
+      <c r="H19" s="81"/>
+      <c r="I19" s="81"/>
+      <c r="J19" s="81"/>
+      <c r="K19" s="81"/>
+      <c r="L19" s="81"/>
+      <c r="M19" s="81"/>
+      <c r="N19" s="81"/>
+      <c r="O19" s="82"/>
       <c r="P19" s="51"/>
       <c r="Q19" s="51"/>
       <c r="R19" s="51"/>
@@ -9135,8 +9135,12 @@
       <c r="E20" s="2">
         <v>-30</v>
       </c>
-      <c r="F20" s="2"/>
-      <c r="G20" s="40"/>
+      <c r="F20" s="2">
+        <v>-17</v>
+      </c>
+      <c r="G20" s="40">
+        <v>-14</v>
+      </c>
       <c r="H20" s="7">
         <v>11</v>
       </c>
@@ -9146,19 +9150,23 @@
       <c r="J20" s="2">
         <v>17</v>
       </c>
-      <c r="K20" s="2"/>
-      <c r="L20" s="41"/>
+      <c r="K20" s="2">
+        <v>34</v>
+      </c>
+      <c r="L20" s="41">
+        <v>8</v>
+      </c>
       <c r="M20" s="7">
         <f>SUM(C20:G20)/5</f>
-        <v>-8.1999999999999993</v>
+        <v>-14.4</v>
       </c>
       <c r="N20" s="44">
         <f>SUM(H20:L20)/5</f>
-        <v>8</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="O20" s="48">
         <f t="shared" si="2"/>
-        <v>11.456002793295749</v>
+        <v>21.824756585125982</v>
       </c>
       <c r="P20" s="58">
         <f t="shared" si="7"/>
@@ -9174,17 +9182,17 @@
       </c>
       <c r="S20" s="59">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>38.013155617496423</v>
       </c>
       <c r="T20" s="59">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>16.124515496597098</v>
       </c>
       <c r="U20" s="60">
         <f t="shared" si="12"/>
-        <v>12.002368677054999</v>
-      </c>
-      <c r="X20" s="90">
+        <v>22.829902899873705</v>
+      </c>
+      <c r="X20" s="62">
         <v>4.3055555555555562E-2</v>
       </c>
       <c r="AC20">
@@ -9465,22 +9473,22 @@
       <c r="AN23" s="51"/>
     </row>
     <row r="24" spans="2:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="67" t="s">
+      <c r="B24" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="68"/>
-      <c r="D24" s="68"/>
-      <c r="E24" s="68"/>
-      <c r="F24" s="68"/>
-      <c r="G24" s="68"/>
-      <c r="H24" s="68"/>
-      <c r="I24" s="68"/>
-      <c r="J24" s="68"/>
-      <c r="K24" s="68"/>
-      <c r="L24" s="68"/>
-      <c r="M24" s="68"/>
-      <c r="N24" s="68"/>
-      <c r="O24" s="69"/>
+      <c r="C24" s="81"/>
+      <c r="D24" s="81"/>
+      <c r="E24" s="81"/>
+      <c r="F24" s="81"/>
+      <c r="G24" s="81"/>
+      <c r="H24" s="81"/>
+      <c r="I24" s="81"/>
+      <c r="J24" s="81"/>
+      <c r="K24" s="81"/>
+      <c r="L24" s="81"/>
+      <c r="M24" s="81"/>
+      <c r="N24" s="81"/>
+      <c r="O24" s="82"/>
       <c r="P24" s="51"/>
       <c r="Q24" s="51"/>
       <c r="R24" s="51"/>
@@ -9573,7 +9581,7 @@
         <f t="shared" si="12"/>
         <v>15.875485687217978</v>
       </c>
-      <c r="W25" s="90">
+      <c r="W25" s="62">
         <v>6.8749999999999992E-2</v>
       </c>
       <c r="AC25">
@@ -9876,22 +9884,22 @@
       </c>
     </row>
     <row r="29" spans="2:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="67" t="s">
+      <c r="B29" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="68"/>
-      <c r="D29" s="68"/>
-      <c r="E29" s="68"/>
-      <c r="F29" s="68"/>
-      <c r="G29" s="68"/>
-      <c r="H29" s="68"/>
-      <c r="I29" s="68"/>
-      <c r="J29" s="68"/>
-      <c r="K29" s="68"/>
-      <c r="L29" s="68"/>
-      <c r="M29" s="68"/>
-      <c r="N29" s="68"/>
-      <c r="O29" s="69"/>
+      <c r="C29" s="81"/>
+      <c r="D29" s="81"/>
+      <c r="E29" s="81"/>
+      <c r="F29" s="81"/>
+      <c r="G29" s="81"/>
+      <c r="H29" s="81"/>
+      <c r="I29" s="81"/>
+      <c r="J29" s="81"/>
+      <c r="K29" s="81"/>
+      <c r="L29" s="81"/>
+      <c r="M29" s="81"/>
+      <c r="N29" s="81"/>
+      <c r="O29" s="82"/>
       <c r="P29" s="51"/>
       <c r="Q29" s="51"/>
       <c r="R29" s="51"/>
@@ -9907,51 +9915,74 @@
       <c r="B30" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="C30" s="7"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="41"/>
+      <c r="C30" s="7">
+        <v>-8</v>
+      </c>
+      <c r="D30" s="2">
+        <v>-12</v>
+      </c>
+      <c r="E30" s="2">
+        <v>-6</v>
+      </c>
+      <c r="F30" s="2">
+        <v>-11</v>
+      </c>
+      <c r="G30" s="40">
+        <v>7</v>
+      </c>
+      <c r="H30" s="7">
+        <v>14</v>
+      </c>
+      <c r="I30" s="2">
+        <v>19</v>
+      </c>
+      <c r="J30" s="2">
+        <v>15</v>
+      </c>
+      <c r="K30" s="2">
+        <v>11</v>
+      </c>
+      <c r="L30" s="41">
+        <v>-9</v>
+      </c>
       <c r="M30" s="7">
         <f>SUM(C30:G30)/5</f>
-        <v>0</v>
+        <v>-6</v>
       </c>
       <c r="N30" s="44">
         <f>SUM(H30:L30)/5</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="O30" s="55">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>11.661903789690601</v>
       </c>
       <c r="P30" s="58">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>16.124515496597098</v>
       </c>
       <c r="Q30" s="59">
         <f>SQRT((D30)^2+(I30)^2)</f>
-        <v>0</v>
+        <v>22.472205054244231</v>
       </c>
       <c r="R30" s="59">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>16.15549442140351</v>
       </c>
       <c r="S30" s="59">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>15.556349186104045</v>
       </c>
       <c r="T30" s="59">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>11.401754250991379</v>
       </c>
       <c r="U30" s="60">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>16.342063681868051</v>
+      </c>
+      <c r="W30" s="62">
+        <v>0.11875000000000001</v>
       </c>
       <c r="AC30">
         <v>0.25</v>
@@ -10242,22 +10273,22 @@
       <c r="AP33" s="51"/>
     </row>
     <row r="34" spans="2:42" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="64" t="s">
+      <c r="B34" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="C34" s="65"/>
-      <c r="D34" s="65"/>
-      <c r="E34" s="65"/>
-      <c r="F34" s="65"/>
-      <c r="G34" s="65"/>
-      <c r="H34" s="65"/>
-      <c r="I34" s="65"/>
-      <c r="J34" s="65"/>
-      <c r="K34" s="65"/>
-      <c r="L34" s="65"/>
-      <c r="M34" s="65"/>
-      <c r="N34" s="65"/>
-      <c r="O34" s="66"/>
+      <c r="C34" s="78"/>
+      <c r="D34" s="78"/>
+      <c r="E34" s="78"/>
+      <c r="F34" s="78"/>
+      <c r="G34" s="78"/>
+      <c r="H34" s="78"/>
+      <c r="I34" s="78"/>
+      <c r="J34" s="78"/>
+      <c r="K34" s="78"/>
+      <c r="L34" s="78"/>
+      <c r="M34" s="78"/>
+      <c r="N34" s="78"/>
+      <c r="O34" s="79"/>
       <c r="AJ34">
         <v>0.5</v>
       </c>
@@ -10461,14 +10492,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="V2:V9"/>
-    <mergeCell ref="U2:U9"/>
-    <mergeCell ref="P2:T2"/>
-    <mergeCell ref="P3:P9"/>
-    <mergeCell ref="Q3:Q9"/>
-    <mergeCell ref="R3:R9"/>
-    <mergeCell ref="S3:S9"/>
-    <mergeCell ref="T3:T9"/>
     <mergeCell ref="O2:O3"/>
     <mergeCell ref="B34:O34"/>
     <mergeCell ref="B29:O29"/>
@@ -10482,6 +10505,14 @@
     <mergeCell ref="C2:G2"/>
     <mergeCell ref="H2:L2"/>
     <mergeCell ref="M2:M3"/>
+    <mergeCell ref="V2:V9"/>
+    <mergeCell ref="U2:U9"/>
+    <mergeCell ref="P2:T2"/>
+    <mergeCell ref="P3:P9"/>
+    <mergeCell ref="Q3:Q9"/>
+    <mergeCell ref="R3:R9"/>
+    <mergeCell ref="S3:S9"/>
+    <mergeCell ref="T3:T9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>